<commit_message>
Update CLUB VIDEO Jeu d'essai.xlsx
</commit_message>
<xml_diff>
--- a/103_BaseDeDonnees/Exercices/204_ClubVideo/CLUB VIDEO Jeu d'essai.xlsx
+++ b/103_BaseDeDonnees/Exercices/204_ClubVideo/CLUB VIDEO Jeu d'essai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcravo\Documents\GitHub\FORMATION-CDA-2210\103_BaseDeDonnees\Exercices\204_ClubVideo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DD44BB-4F2F-4508-B821-36BCEEE5FEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD183E4-6AC9-4DEC-AEBD-2589C53EAAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26955" yWindow="1545" windowWidth="18900" windowHeight="11055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="7980" windowWidth="12900" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nominatifs" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
   <si>
     <t>Prenom</t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>Hors-Circuits</t>
+  </si>
+  <si>
+    <t>acteur</t>
+  </si>
+  <si>
+    <t>réalisateur</t>
+  </si>
+  <si>
+    <t>client</t>
   </si>
 </sst>
 </file>
@@ -599,183 +608,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -787,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1063AB25-8800-4323-B883-AF54ECA968BD}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>